<commit_message>
ZWS-12 Charts in XLSX
</commit_message>
<xml_diff>
--- a/output_analysis.xlsx
+++ b/output_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hg/pwr/7sem/zwsisk/proj-wojcik/page-replacement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEEB148-D94F-574C-B132-9EBE2BFD28B0}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE445632-A6E8-044C-B2AA-D6C970F42297}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BF315AA1-11C1-4F4D-A6A8-88A9E7B68DA2}"/>
   </bookViews>
@@ -25,6 +25,38 @@
     <definedName name="_64_frames" localSheetId="0">Arkusz1!$A$10:$H$13</definedName>
     <definedName name="_64_frames_1" localSheetId="0">Arkusz1!$A$22:$H$25</definedName>
     <definedName name="_64_frames_2" localSheetId="0">Arkusz1!$A$34:$H$37</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">(Arkusz1!$C$2,Arkusz1!$C$6,Arkusz1!$C$10)</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">(Arkusz1!$C$3,Arkusz1!$C$7,Arkusz1!$C$11)</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">(Arkusz1!$C$2,Arkusz1!$C$6,Arkusz1!$C$10)</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">(Arkusz1!$C$3,Arkusz1!$C$7,Arkusz1!$C$11)</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">(Arkusz1!$C$4,Arkusz1!$C$8,Arkusz1!$C$12)</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">(Arkusz1!$E$2,Arkusz1!$E$6,Arkusz1!$E$10)</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">(Arkusz1!$E$3,Arkusz1!$E$7,Arkusz1!$E$11)</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">(Arkusz1!$E$4,Arkusz1!$E$8,Arkusz1!$E$12)</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">(Arkusz1!$C$2,Arkusz1!$C$6,Arkusz1!$C$10)</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">(Arkusz1!$C$3,Arkusz1!$C$7,Arkusz1!$C$11)</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">(Arkusz1!$C$4,Arkusz1!$C$8,Arkusz1!$C$12)</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">(Arkusz1!$E$2,Arkusz1!$E$6,Arkusz1!$E$10)</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">(Arkusz1!$C$4,Arkusz1!$C$8,Arkusz1!$C$12)</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">(Arkusz1!$E$3,Arkusz1!$E$7,Arkusz1!$E$11)</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">(Arkusz1!$E$4,Arkusz1!$E$8,Arkusz1!$E$12)</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">(Arkusz1!$C$2,Arkusz1!$C$6,Arkusz1!$C$10)</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">(Arkusz1!$C$3,Arkusz1!$C$7,Arkusz1!$C$11)</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">(Arkusz1!$E$2,Arkusz1!$E$6,Arkusz1!$E$10)</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">(Arkusz1!$E$3,Arkusz1!$E$7,Arkusz1!$E$11)</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">(Arkusz1!$C$2,Arkusz1!$C$6,Arkusz1!$C$10)</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">(Arkusz1!$C$3,Arkusz1!$C$7,Arkusz1!$C$11)</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">(Arkusz1!$C$4,Arkusz1!$C$8,Arkusz1!$C$12)</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">(Arkusz1!$E$2,Arkusz1!$E$6,Arkusz1!$E$10)</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">(Arkusz1!$E$2,Arkusz1!$E$6,Arkusz1!$E$10)</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">(Arkusz1!$E$3,Arkusz1!$E$7,Arkusz1!$E$11)</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">(Arkusz1!$E$4,Arkusz1!$E$8,Arkusz1!$E$12)</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">(Arkusz1!$E$3,Arkusz1!$E$7,Arkusz1!$E$11)</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">(Arkusz1!$E$4,Arkusz1!$E$8,Arkusz1!$E$12)</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">(Arkusz1!$C$2,Arkusz1!$C$6,Arkusz1!$C$10)</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">(Arkusz1!$C$3,Arkusz1!$C$7,Arkusz1!$C$11)</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">(Arkusz1!$E$2,Arkusz1!$E$6,Arkusz1!$E$10)</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">(Arkusz1!$E$3,Arkusz1!$E$7,Arkusz1!$E$11)</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -376,6 +408,4419 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="0" baseline="0">
+                <a:gradFill>
+                  <a:gsLst>
+                    <a:gs pos="0">
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:gs>
+                    <a:gs pos="100000">
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="85000"/>
+                        <a:lumOff val="15000"/>
+                      </a:schemeClr>
+                    </a:gs>
+                  </a:gsLst>
+                  <a:lin ang="5400000" scaled="0"/>
+                </a:gradFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>100000.trace</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="0" baseline="0">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="85000"/>
+                      <a:lumOff val="15000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Clock</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="17"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Arkusz1!$C$5,Arkusz1!$C$9,Arkusz1!$C$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Arkusz1!$E$2,Arkusz1!$E$6,Arkusz1!$E$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>89458</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>78928</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57494</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-89AF-184B-BF1E-8A1E8CF4C13D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>LRU</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="17"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="accent5"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Arkusz1!$C$5,Arkusz1!$C$9,Arkusz1!$C$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Arkusz1!$E$3,Arkusz1!$E$7,Arkusz1!$E$11)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>89528</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>78903</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57698</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-89AF-184B-BF1E-8A1E8CF4C13D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Aging</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="17"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Arkusz1!$C$5,Arkusz1!$C$9,Arkusz1!$C$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Arkusz1!$E$4,Arkusz1!$E$8,Arkusz1!$E$12)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>89625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>78826</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57698</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-89AF-184B-BF1E-8A1E8CF4C13D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Opt</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="17"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Arkusz1!$C$5,Arkusz1!$C$9,Arkusz1!$C$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Arkusz1!$E$5,Arkusz1!$E$9,Arkusz1!$E$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>71564</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60220</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43118</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-89AF-184B-BF1E-8A1E8CF4C13D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1068182079"/>
+        <c:axId val="1067950927"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1068182079"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Ramki</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1067950927"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1067950927"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Błędy stron</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1068182079"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="0" baseline="0">
+                <a:gradFill>
+                  <a:gsLst>
+                    <a:gs pos="0">
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:gs>
+                    <a:gs pos="100000">
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="85000"/>
+                        <a:lumOff val="15000"/>
+                      </a:schemeClr>
+                    </a:gs>
+                  </a:gsLst>
+                  <a:lin ang="5400000" scaled="0"/>
+                </a:gradFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>200000.trace</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="0" baseline="0">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="85000"/>
+                      <a:lumOff val="15000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Clock</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="17"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Arkusz1!$C$5,Arkusz1!$C$9,Arkusz1!$C$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Arkusz1!$E$14,Arkusz1!$E$18,Arkusz1!$E$22)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>223409</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>196960</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>144245</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4245-6643-A247-AD91DE18CA30}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>LRU</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="17"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="accent5"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Arkusz1!$C$5,Arkusz1!$C$9,Arkusz1!$C$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Arkusz1!$E$15,Arkusz1!$E$19,Arkusz1!$E$23)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>223394</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>196899</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>143774</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4245-6643-A247-AD91DE18CA30}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Aging</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="17"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Arkusz1!$C$5,Arkusz1!$C$9,Arkusz1!$C$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Arkusz1!$E$16,Arkusz1!$E$20,Arkusz1!$E$24)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>223413</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>197050</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>143999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4245-6643-A247-AD91DE18CA30}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Opt</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="17"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Arkusz1!$C$5,Arkusz1!$C$9,Arkusz1!$C$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Arkusz1!$E$17,Arkusz1!$E$21,Arkusz1!$E$25)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>178583</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>150162</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>108061</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-4245-6643-A247-AD91DE18CA30}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1068182079"/>
+        <c:axId val="1067950927"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1068182079"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Ramki</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1067950927"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1067950927"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Błędy stron</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1068182079"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="0" baseline="0">
+                <a:gradFill>
+                  <a:gsLst>
+                    <a:gs pos="0">
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:gs>
+                    <a:gs pos="100000">
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="85000"/>
+                        <a:lumOff val="15000"/>
+                      </a:schemeClr>
+                    </a:gs>
+                  </a:gsLst>
+                  <a:lin ang="5400000" scaled="0"/>
+                </a:gradFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>500000.trace</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="0" baseline="0">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="85000"/>
+                      <a:lumOff val="15000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Clock</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="17"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Arkusz1!$C$5,Arkusz1!$C$9,Arkusz1!$C$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Arkusz1!$E$26,Arkusz1!$E$30,Arkusz1!$E$34)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>447049</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>394365</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>288494</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1A6B-9249-8062-EDBC08253925}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>LRU</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="17"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="accent5"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Arkusz1!$C$5,Arkusz1!$C$9,Arkusz1!$C$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Arkusz1!$E$27,Arkusz1!$E$31,Arkusz1!$E$35)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>447339</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>394257</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>287688</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1A6B-9249-8062-EDBC08253925}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Aging</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="17"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Arkusz1!$C$5,Arkusz1!$C$9,Arkusz1!$C$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Arkusz1!$E$28,Arkusz1!$E$32,Arkusz1!$E$36)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>447146</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>394464</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>288347</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1A6B-9249-8062-EDBC08253925}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Opt</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="17"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Arkusz1!$C$5,Arkusz1!$C$9,Arkusz1!$C$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Arkusz1!$E$29,Arkusz1!$E$33,Arkusz1!$E$37)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>357466</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300668</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>215641</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-1A6B-9249-8062-EDBC08253925}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1068182079"/>
+        <c:axId val="1067950927"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1068182079"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Ramki</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1067950927"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1067950927"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Błędy stron</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1068182079"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="234">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr/>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9575">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+            <a:satMod val="105000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="17"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1440" b="0" kern="1200" cap="all" spc="0" baseline="0">
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="234">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr/>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9575">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+            <a:satMod val="105000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="17"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1440" b="0" kern="1200" cap="all" spc="0" baseline="0">
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="234">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr/>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9575">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+            <a:satMod val="105000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="17"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1440" b="0" kern="1200" cap="all" spc="0" baseline="0">
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>192424</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>12828</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Wykres 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF3B5B16-57D8-7E43-BCF8-9F37350EE713}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1423939</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>12828</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>808180</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>38485</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Wykres 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37567F51-552F-E54C-8A12-831F8E0D5304}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>821009</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>25657</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Wykres 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C27D4DB8-2B40-E047-A723-70886339A69C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -713,8 +5158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAFDEB2E-202E-1346-AE0D-E25D4AD48539}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1695,5 +6140,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>